<commit_message>
Implement markov approach for eThRampUp/Dw
Add separate flag in Power_Parameters to switch edge handling for ramping constraints
Also adjust secondReserve formulation accordingly
</commit_message>
<xml_diff>
--- a/data/markov/Power_Parameters.xlsx
+++ b/data/markov/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BA0B06-F2D1-4AE9-A85F-241B5D081D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E353F-8075-468B-812B-895E0F1A8B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12645" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="151">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -453,9 +453,6 @@
     <t>[notEnforced, cyclic, markov]</t>
   </si>
   <si>
-    <t>Minimum Up-/Down Time</t>
-  </si>
-  <si>
     <t>markov</t>
   </si>
   <si>
@@ -501,13 +498,25 @@
     <t>Enable Import/Export, requires Power_ImpExpHubs.xlsx and Power_ImpExpProfiles.xlsx files</t>
   </si>
   <si>
-    <t>Constraint enforce type for edge timesteps within p</t>
-  </si>
-  <si>
     <t>How should constraints be enforced at edges of repr. periods. Either, not enforced (=notEnforced), cyclically or using markov chains (from the transition matrix, which also means relaxing the binary form of affected variables)</t>
   </si>
   <si>
     <t>pReprPeriodEdgeHandlingUnitCommitment</t>
+  </si>
+  <si>
+    <t>Edge handling</t>
+  </si>
+  <si>
+    <t>pReprPeriodEdgeHandlingRamping</t>
+  </si>
+  <si>
+    <t>Ramping constraint type for edge timesteps within p</t>
+  </si>
+  <si>
+    <t>Unit Commitment constraint type for edge timesteps</t>
+  </si>
+  <si>
+    <t>How should constraints be enforced at edges of repr. periods. Either, not enforced (=notEnforced), cyclically or using markov chains (from the transition matrix)</t>
   </si>
 </sst>
 </file>
@@ -725,495 +734,509 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
       </font>
     </dxf>
   </dxfs>
@@ -1533,10 +1556,10 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H141"/>
+  <dimension ref="B1:H144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1681,12 +1704,12 @@
     </row>
     <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>54</v>
@@ -1694,13 +1717,13 @@
     </row>
     <row r="18" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1709,7 +1732,7 @@
     </row>
     <row r="20" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>54</v>
@@ -1717,13 +1740,13 @@
     </row>
     <row r="21" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1732,7 +1755,7 @@
     </row>
     <row r="23" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>54</v>
@@ -1740,13 +1763,13 @@
     </row>
     <row r="24" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1755,7 +1778,7 @@
     </row>
     <row r="26" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>54</v>
@@ -1763,13 +1786,13 @@
     </row>
     <row r="27" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1792,7 +1815,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,12 +2502,12 @@
     </row>
     <row r="139" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="7" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="140" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C140" s="8" t="s">
         <v>128</v>
@@ -2492,28 +2515,58 @@
     </row>
     <row r="141" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>128</v>
       </c>
     </row>
+    <row r="143" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B143" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B144" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="69" priority="38" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="37" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
+    <cfRule type="cellIs" dxfId="69" priority="100" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="99" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C12">
     <cfRule type="cellIs" dxfId="67" priority="98" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2521,31 +2574,31 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="65" priority="96" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="95" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C14:C31">
-    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="61" priority="108" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="110" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="109" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40 C43">
     <cfRule type="cellIs" dxfId="59" priority="86" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2553,7 +2606,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40 C43">
+  <conditionalFormatting sqref="C46">
     <cfRule type="cellIs" dxfId="57" priority="84" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2561,7 +2614,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C49">
     <cfRule type="cellIs" dxfId="55" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2569,7 +2622,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="53" priority="80" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2577,7 +2630,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C56">
     <cfRule type="cellIs" dxfId="51" priority="78" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2585,7 +2638,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C59">
     <cfRule type="cellIs" dxfId="49" priority="76" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2593,7 +2646,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C63">
     <cfRule type="cellIs" dxfId="47" priority="74" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2601,15 +2654,15 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="45" priority="71" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="72" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C66">
+    <cfRule type="cellIs" dxfId="45" priority="72" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="71" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
     <cfRule type="cellIs" dxfId="43" priority="70" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2617,15 +2670,15 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="41" priority="68" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="67" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C72">
+    <cfRule type="cellIs" dxfId="41" priority="67" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="68" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
     <cfRule type="cellIs" dxfId="39" priority="66" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2633,55 +2686,55 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="37" priority="64" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="63" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="35" priority="61" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="63" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="64" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="33" priority="59" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="60" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="35" priority="62" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="61" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="31" priority="57" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="58" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="60" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="59" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="29" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="56" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="31" priority="58" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="57" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="cellIs" dxfId="27" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
+    <cfRule type="cellIs" dxfId="27" priority="53" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101:C102">
     <cfRule type="cellIs" dxfId="25" priority="52" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2689,47 +2742,47 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C101:C102">
-    <cfRule type="cellIs" dxfId="23" priority="50" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="49" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="19" priority="48" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="50" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="49" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="17" priority="33" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="35" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="36" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114 C117">
-    <cfRule type="cellIs" dxfId="15" priority="42" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="43" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121">
+    <cfRule type="cellIs" dxfId="15" priority="48" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="47" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C124">
     <cfRule type="cellIs" dxfId="13" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2737,39 +2790,39 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C124">
-    <cfRule type="cellIs" dxfId="11" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C128:C129">
-    <cfRule type="cellIs" dxfId="9" priority="92" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="94" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="93" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C131:C132">
-    <cfRule type="cellIs" dxfId="7" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="31" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C134:C135">
-    <cfRule type="cellIs" dxfId="5" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C137:C138">
+    <cfRule type="cellIs" dxfId="5" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="23" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C141">
     <cfRule type="cellIs" dxfId="3" priority="22" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2777,20 +2830,20 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C141">
-    <cfRule type="cellIs" dxfId="1" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="equal">
-      <formula>"No"</formula>
+  <conditionalFormatting sqref="C144">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C34 C37 C46 C59 C63 C81 C97 C108 C121 C124 C101:C102 C114 C117 C30 C18 C21 C24 C27" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C129 C132 C135 C138 C15:C16 C17:C31" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C128 C77 C49 C56 C131 C134 C137 C141" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C129 C132 C135 C138 C15:C31" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C128 C77 C49 C56 C131 C134 C137 C141 C144" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2807,6 +2860,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2952,12 +3011,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2967,6 +3020,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2982,20 +3051,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add plot for PNS & EPS
Adjust markov case to remove PNS
Make saving to sqlite optional
</commit_message>
<xml_diff>
--- a/data/markov/Power_Parameters.xlsx
+++ b/data/markov/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\markov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985FE18A-9879-4590-98B0-04E4B483423D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B928E019-F8BB-4491-B95E-C8B0F6395F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50190" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -1098,7 +1098,9 @@
   </sheetPr>
   <dimension ref="B1:H76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1535,7 +1537,7 @@
         <v>6</v>
       </c>
       <c r="C60" s="10">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>17</v>
@@ -1564,7 +1566,7 @@
         <v>66</v>
       </c>
       <c r="C63" s="10">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>37</v>
@@ -1829,12 +1831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1980,6 +1976,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1990,22 +1992,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2023,6 +2009,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>